<commit_message>
Add expanded nodes and path tables
</commit_message>
<xml_diff>
--- a/docs/time_analysis.xlsx
+++ b/docs/time_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U. Porto\3 ano\2 semestre\IART-g39\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B5A3D4-CF9E-4DAF-AA62-E68FC17CDB00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EC6BD6-1E3A-4981-8CFD-CD8098EC79DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{80728A2F-030A-4331-A84E-3313CB5F0CBB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{80728A2F-030A-4331-A84E-3313CB5F0CBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
   <si>
     <t>Level 1</t>
   </si>
@@ -114,12 +114,21 @@
   <si>
     <t>Iterative Deepening</t>
   </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Path Size</t>
+  </si>
+  <si>
+    <t>Expanded Nodes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,13 +150,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -297,9 +320,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -316,6 +338,11 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1578,7 +1605,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$8</c15:sqref>
@@ -1607,7 +1634,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -1681,7 +1708,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$8:$V$8</c15:sqref>
@@ -1755,7 +1782,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-B7AE-428E-A3B7-CADB51C3FE80}"/>
                   </c:ext>
@@ -1768,7 +1795,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$9</c15:sqref>
@@ -1797,7 +1824,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -1871,7 +1898,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$9:$V$9</c15:sqref>
@@ -1945,7 +1972,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-B7AE-428E-A3B7-CADB51C3FE80}"/>
                   </c:ext>
@@ -2834,7 +2861,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$6</c15:sqref>
@@ -2863,7 +2890,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -2937,7 +2964,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$6:$V$6</c15:sqref>
@@ -3011,7 +3038,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-5698-44C8-8425-C353708BDC28}"/>
                   </c:ext>
@@ -3024,7 +3051,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$8</c15:sqref>
@@ -3053,7 +3080,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -3127,7 +3154,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$8:$V$8</c15:sqref>
@@ -3201,7 +3228,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-5698-44C8-8425-C353708BDC28}"/>
                   </c:ext>
@@ -3214,7 +3241,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$9</c15:sqref>
@@ -3243,7 +3270,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -3317,7 +3344,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$9:$V$9</c15:sqref>
@@ -3391,7 +3418,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-5698-44C8-8425-C353708BDC28}"/>
                   </c:ext>
@@ -5902,7 +5929,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$5</c15:sqref>
@@ -5931,7 +5958,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -6005,7 +6032,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$5:$V$5</c15:sqref>
@@ -6079,7 +6106,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-A1BA-408B-AC70-7069384A41A6}"/>
                   </c:ext>
@@ -6092,7 +6119,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$7</c15:sqref>
@@ -6121,7 +6148,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -6195,7 +6222,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$7:$V$7</c15:sqref>
@@ -6269,7 +6296,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-A1BA-408B-AC70-7069384A41A6}"/>
                   </c:ext>
@@ -6282,7 +6309,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$8</c15:sqref>
@@ -6311,7 +6338,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -6385,7 +6412,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$8:$V$8</c15:sqref>
@@ -6459,7 +6486,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-A1BA-408B-AC70-7069384A41A6}"/>
                   </c:ext>
@@ -7121,7 +7148,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$5</c15:sqref>
@@ -7150,7 +7177,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -7224,7 +7251,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$5:$V$5</c15:sqref>
@@ -7298,7 +7325,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-9523-45B5-92D6-608375F5BC24}"/>
                   </c:ext>
@@ -7311,7 +7338,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$6</c15:sqref>
@@ -7340,7 +7367,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -7414,7 +7441,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$6:$V$6</c15:sqref>
@@ -7488,7 +7515,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-9523-45B5-92D6-608375F5BC24}"/>
                   </c:ext>
@@ -7501,7 +7528,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$8</c15:sqref>
@@ -7530,7 +7557,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -7604,7 +7631,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$8:$V$8</c15:sqref>
@@ -7678,7 +7705,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000C-9523-45B5-92D6-608375F5BC24}"/>
                   </c:ext>
@@ -8340,7 +8367,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$5</c15:sqref>
@@ -8369,7 +8396,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -8443,7 +8470,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$5:$V$5</c15:sqref>
@@ -8517,7 +8544,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-0303-4FF2-A58D-32164C3D393E}"/>
                   </c:ext>
@@ -8530,7 +8557,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$6</c15:sqref>
@@ -8559,7 +8586,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -8633,7 +8660,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$6:$V$6</c15:sqref>
@@ -8707,7 +8734,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-0303-4FF2-A58D-32164C3D393E}"/>
                   </c:ext>
@@ -8720,7 +8747,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$7</c15:sqref>
@@ -8749,7 +8776,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -8823,7 +8850,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$7:$V$7</c15:sqref>
@@ -8897,7 +8924,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-0303-4FF2-A58D-32164C3D393E}"/>
                   </c:ext>
@@ -9759,7 +9786,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$6</c15:sqref>
@@ -9788,7 +9815,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -9862,7 +9889,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$6:$V$6</c15:sqref>
@@ -9936,7 +9963,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-85E4-4CA0-B159-1C331441A099}"/>
                   </c:ext>
@@ -9949,7 +9976,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$7</c15:sqref>
@@ -9978,7 +10005,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -10052,7 +10079,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$7:$V$7</c15:sqref>
@@ -10126,7 +10153,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-85E4-4CA0-B159-1C331441A099}"/>
                   </c:ext>
@@ -10139,7 +10166,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$8</c15:sqref>
@@ -10168,7 +10195,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -10242,7 +10269,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$8:$V$8</c15:sqref>
@@ -10316,7 +10343,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-85E4-4CA0-B159-1C331441A099}"/>
                   </c:ext>
@@ -12366,7 +12393,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$5</c15:sqref>
@@ -12395,7 +12422,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -12469,7 +12496,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$5:$V$5</c15:sqref>
@@ -12543,7 +12570,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-A05C-48AA-927D-1EC927D326E4}"/>
                   </c:ext>
@@ -12556,7 +12583,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$6</c15:sqref>
@@ -12585,7 +12612,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -12659,7 +12686,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$6:$V$6</c15:sqref>
@@ -12733,7 +12760,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-A05C-48AA-927D-1EC927D326E4}"/>
                   </c:ext>
@@ -12746,7 +12773,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$7</c15:sqref>
@@ -12775,7 +12802,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -12849,7 +12876,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$7:$V$7</c15:sqref>
@@ -12923,7 +12950,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-A05C-48AA-927D-1EC927D326E4}"/>
                   </c:ext>
@@ -12936,7 +12963,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$B$8</c15:sqref>
@@ -12965,7 +12992,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$3:$V$3</c15:sqref>
@@ -13039,7 +13066,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Dados!$C$8:$V$8</c15:sqref>
@@ -13113,7 +13140,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-A05C-48AA-927D-1EC927D326E4}"/>
                   </c:ext>
@@ -20156,10 +20183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8F887B-5E63-41C2-AD6C-350EA53EFBC0}">
-  <dimension ref="B2:V10"/>
+  <dimension ref="B2:V30"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:V9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20169,459 +20196,1375 @@
   <sheetData>
     <row r="2" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="1"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="V3" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>1.011E-3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>9.9799999999999997E-4</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>2E-3</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>2E-3</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>2E-3</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>2E-3</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="1">
         <v>4.0010000000000002E-3</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <v>1.8651000000000001E-2</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
         <v>2.006E-3</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="1">
         <v>3.045E-3</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="1">
         <v>1.9970000000000001E-3</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="1">
         <v>1.9989999999999999E-3</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="1">
         <v>5.0470000000000003E-3</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="1">
         <v>6.9959999999999996E-3</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="1">
         <v>7.0460000000000002E-3</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4" s="1">
         <v>8.5869999999999991E-3</v>
       </c>
-      <c r="V4" s="7">
+      <c r="V4" s="6">
         <v>0.01</v>
       </c>
     </row>
     <row r="5" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>9.9299999999999996E-4</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>1E-3</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>1.0009999999999999E-3</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>2.9989999999999999E-3</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>3.999E-3</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>1E-3</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>3.0010000000000002E-3</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="1">
         <v>1.6046999999999999E-2</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="1">
         <v>4.4998999999999997E-2</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="1">
         <v>3.872E-3</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="1">
         <v>5.9940000000000002E-3</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="1">
         <v>1.9559999999999998E-3</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="1">
         <v>2.0089999999999999E-3</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="1">
         <v>7.9559999999999995E-3</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="1">
         <v>8.9529999999999992E-3</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="1">
         <v>1.495E-2</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="1">
         <v>9.9989999999999992E-3</v>
       </c>
-      <c r="V5" s="7">
+      <c r="V5" s="6">
         <v>1.5731999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>9.9599999999999992E-4</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>1E-3</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>2.9979999999999998E-3</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>2E-3</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>3.0010000000000002E-3</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>5.6979999999999999E-3</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="1">
         <v>1.6E-2</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="1">
         <v>4.6524000000000003E-2</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="1">
         <v>3.5490000000000001E-3</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="1">
         <v>5.0020000000000004E-3</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="1">
         <v>3.0479999999999999E-3</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="1">
         <v>9.9099999999999991E-4</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="1">
         <v>7.9979999999999999E-3</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="1">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6" s="1">
         <v>1.4E-2</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6" s="1">
         <v>1.2002000000000001E-2</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V6" s="6">
         <v>1.7003000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>9.9799999999999997E-4</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>1E-3</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>1.9989999999999999E-3</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>6.999E-3</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>2.4E-2</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <v>0.01</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>2.2953000000000001E-2</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="1">
         <v>0.12868599999999999</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="1">
         <v>0.662551</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="1">
         <v>8.9779999999999999E-3</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="1">
         <v>1.6951999999999998E-2</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="1">
         <v>5.0029999999999996E-3</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="1">
         <v>4.9810000000000002E-3</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7" s="1">
         <v>2.9954999999999999E-2</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="1">
         <v>3.2983999999999999E-2</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="1">
         <v>5.4973000000000001E-2</v>
       </c>
-      <c r="U7" s="2">
+      <c r="U7" s="1">
         <v>4.3272999999999999E-2</v>
       </c>
-      <c r="V7" s="7">
+      <c r="V7" s="6">
         <v>6.1940000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>9.9799999999999997E-4</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>2E-3</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>2.9970000000000001E-3</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>6.999E-3</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>3.6997000000000002E-2</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <v>0.144903</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>0.13766500000000001</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="1">
         <v>0.42546</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="1">
         <v>1.8493630000000001</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="1">
         <v>0.82670299999999997</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="1">
         <v>0.76427299999999998</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="1">
         <v>0.43917099999999998</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8" s="1">
         <v>0.35388399999999998</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" s="1">
         <v>10.221049000000001</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8" s="1">
         <v>12.021041</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="1">
         <v>18.215354999999999</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8" s="1">
         <v>40.585777</v>
       </c>
-      <c r="V8" s="7">
+      <c r="V8" s="6">
         <v>111.457792</v>
       </c>
     </row>
     <row r="9" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>1.0009999999999999E-3</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>1E-3</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>1.9970000000000001E-3</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>2E-3</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>1.9989999999999999E-3</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>3.999E-3</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="2">
         <v>5.8739999999999999E-3</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>1.6001000000000001E-2</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="2">
         <v>4.7508000000000002E-2</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <v>3.0010000000000002E-3</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="2">
         <v>4.999E-3</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="2">
         <v>1.9970000000000001E-3</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="Q9" s="2">
         <v>2.0019999999999999E-3</v>
       </c>
-      <c r="R9" s="3">
+      <c r="R9" s="2">
         <v>8.0009999999999994E-3</v>
       </c>
-      <c r="S9" s="3">
+      <c r="S9" s="2">
         <v>9.0030000000000006E-3</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9" s="2">
         <v>1.4E-2</v>
       </c>
-      <c r="U9" s="3">
+      <c r="U9" s="2">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="V9" s="9">
+      <c r="V9" s="8">
         <v>1.6997000000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1">
+        <v>6</v>
+      </c>
+      <c r="H14" s="1">
+        <v>7</v>
+      </c>
+      <c r="I14" s="1">
+        <v>7</v>
+      </c>
+      <c r="J14" s="1">
+        <v>8</v>
+      </c>
+      <c r="K14" s="1">
+        <v>8</v>
+      </c>
+      <c r="L14" s="1">
+        <v>8</v>
+      </c>
+      <c r="M14" s="1">
+        <v>9</v>
+      </c>
+      <c r="N14" s="1">
+        <v>10</v>
+      </c>
+      <c r="O14" s="1">
+        <v>10</v>
+      </c>
+      <c r="P14" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>11</v>
+      </c>
+      <c r="R14" s="1">
+        <v>12</v>
+      </c>
+      <c r="S14" s="1">
+        <v>13</v>
+      </c>
+      <c r="T14" s="1">
+        <v>13</v>
+      </c>
+      <c r="U14" s="1">
+        <v>14</v>
+      </c>
+      <c r="V14" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1">
+        <v>6</v>
+      </c>
+      <c r="H15" s="1">
+        <v>7</v>
+      </c>
+      <c r="I15" s="1">
+        <v>7</v>
+      </c>
+      <c r="J15" s="1">
+        <v>8</v>
+      </c>
+      <c r="K15" s="1">
+        <v>8</v>
+      </c>
+      <c r="L15" s="1">
+        <v>8</v>
+      </c>
+      <c r="M15" s="1">
+        <v>9</v>
+      </c>
+      <c r="N15" s="1">
+        <v>10</v>
+      </c>
+      <c r="O15" s="1">
+        <v>10</v>
+      </c>
+      <c r="P15" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>11</v>
+      </c>
+      <c r="R15" s="1">
+        <v>12</v>
+      </c>
+      <c r="S15" s="1">
+        <v>13</v>
+      </c>
+      <c r="T15" s="1">
+        <v>13</v>
+      </c>
+      <c r="U15" s="1">
+        <v>14</v>
+      </c>
+      <c r="V15" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3</v>
+      </c>
+      <c r="F16" s="1">
+        <v>4</v>
+      </c>
+      <c r="G16" s="1">
+        <v>6</v>
+      </c>
+      <c r="H16" s="1">
+        <v>7</v>
+      </c>
+      <c r="I16" s="1">
+        <v>7</v>
+      </c>
+      <c r="J16" s="1">
+        <v>8</v>
+      </c>
+      <c r="K16" s="1">
+        <v>8</v>
+      </c>
+      <c r="L16" s="1">
+        <v>8</v>
+      </c>
+      <c r="M16" s="1">
+        <v>9</v>
+      </c>
+      <c r="N16" s="1">
+        <v>10</v>
+      </c>
+      <c r="O16" s="1">
+        <v>10</v>
+      </c>
+      <c r="P16" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>11</v>
+      </c>
+      <c r="R16" s="1">
+        <v>12</v>
+      </c>
+      <c r="S16" s="1">
+        <v>13</v>
+      </c>
+      <c r="T16" s="1">
+        <v>13</v>
+      </c>
+      <c r="U16" s="1">
+        <v>14</v>
+      </c>
+      <c r="V16" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4</v>
+      </c>
+      <c r="G17" s="1">
+        <v>6</v>
+      </c>
+      <c r="H17" s="1">
+        <v>7</v>
+      </c>
+      <c r="I17" s="1">
+        <v>7</v>
+      </c>
+      <c r="J17" s="1">
+        <v>8</v>
+      </c>
+      <c r="K17" s="1">
+        <v>8</v>
+      </c>
+      <c r="L17" s="1">
+        <v>8</v>
+      </c>
+      <c r="M17" s="1">
+        <v>9</v>
+      </c>
+      <c r="N17" s="1">
+        <v>10</v>
+      </c>
+      <c r="O17" s="1">
+        <v>10</v>
+      </c>
+      <c r="P17" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>11</v>
+      </c>
+      <c r="R17" s="1">
+        <v>12</v>
+      </c>
+      <c r="S17" s="1">
+        <v>13</v>
+      </c>
+      <c r="T17" s="1">
+        <v>13</v>
+      </c>
+      <c r="U17" s="1">
+        <v>14</v>
+      </c>
+      <c r="V17" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <v>3</v>
+      </c>
+      <c r="F18" s="1">
+        <v>4</v>
+      </c>
+      <c r="G18" s="1">
+        <v>6</v>
+      </c>
+      <c r="H18" s="1">
+        <v>7</v>
+      </c>
+      <c r="I18" s="1">
+        <v>7</v>
+      </c>
+      <c r="J18" s="1">
+        <v>8</v>
+      </c>
+      <c r="K18" s="1">
+        <v>8</v>
+      </c>
+      <c r="L18" s="1">
+        <v>8</v>
+      </c>
+      <c r="M18" s="1">
+        <v>9</v>
+      </c>
+      <c r="N18" s="1">
+        <v>10</v>
+      </c>
+      <c r="O18" s="1">
+        <v>10</v>
+      </c>
+      <c r="P18" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>11</v>
+      </c>
+      <c r="R18" s="1">
+        <v>12</v>
+      </c>
+      <c r="S18" s="1">
+        <v>13</v>
+      </c>
+      <c r="T18" s="1">
+        <v>13</v>
+      </c>
+      <c r="U18" s="1">
+        <v>14</v>
+      </c>
+      <c r="V18" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2">
+        <v>3</v>
+      </c>
+      <c r="F19" s="2">
+        <v>4</v>
+      </c>
+      <c r="G19" s="2">
+        <v>6</v>
+      </c>
+      <c r="H19" s="2">
+        <v>7</v>
+      </c>
+      <c r="I19" s="2">
+        <v>7</v>
+      </c>
+      <c r="J19" s="2">
+        <v>8</v>
+      </c>
+      <c r="K19" s="2">
+        <v>8</v>
+      </c>
+      <c r="L19" s="2">
+        <v>8</v>
+      </c>
+      <c r="M19" s="2">
+        <v>9</v>
+      </c>
+      <c r="N19" s="2">
+        <v>10</v>
+      </c>
+      <c r="O19" s="2">
+        <v>10</v>
+      </c>
+      <c r="P19" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>11</v>
+      </c>
+      <c r="R19" s="2">
+        <v>12</v>
+      </c>
+      <c r="S19" s="2">
+        <v>13</v>
+      </c>
+      <c r="T19" s="2">
+        <v>13</v>
+      </c>
+      <c r="U19" s="2">
+        <v>14</v>
+      </c>
+      <c r="V19" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <v>6</v>
+      </c>
+      <c r="F24" s="1">
+        <v>10</v>
+      </c>
+      <c r="G24" s="1">
+        <v>17</v>
+      </c>
+      <c r="H24" s="1">
+        <v>19</v>
+      </c>
+      <c r="I24" s="1">
+        <v>19</v>
+      </c>
+      <c r="J24" s="1">
+        <v>22</v>
+      </c>
+      <c r="K24" s="1">
+        <v>26</v>
+      </c>
+      <c r="L24" s="1">
+        <v>32</v>
+      </c>
+      <c r="M24" s="1">
+        <v>103</v>
+      </c>
+      <c r="N24" s="1">
+        <v>26</v>
+      </c>
+      <c r="O24" s="1">
+        <v>29</v>
+      </c>
+      <c r="P24" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>18</v>
+      </c>
+      <c r="R24" s="1">
+        <v>37</v>
+      </c>
+      <c r="S24" s="1">
+        <v>52</v>
+      </c>
+      <c r="T24" s="1">
+        <v>44</v>
+      </c>
+      <c r="U24" s="1">
+        <v>57</v>
+      </c>
+      <c r="V24" s="6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1">
+        <v>5</v>
+      </c>
+      <c r="D25" s="11">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1">
+        <v>7</v>
+      </c>
+      <c r="F25" s="1">
+        <v>36</v>
+      </c>
+      <c r="G25" s="1">
+        <v>71</v>
+      </c>
+      <c r="H25" s="1">
+        <v>35</v>
+      </c>
+      <c r="I25" s="1">
+        <v>46</v>
+      </c>
+      <c r="J25" s="1">
+        <v>66</v>
+      </c>
+      <c r="K25" s="1">
+        <v>103</v>
+      </c>
+      <c r="L25" s="1">
+        <v>167</v>
+      </c>
+      <c r="M25" s="1">
+        <v>430</v>
+      </c>
+      <c r="N25" s="1">
+        <v>76</v>
+      </c>
+      <c r="O25" s="1">
+        <v>80</v>
+      </c>
+      <c r="P25" s="1">
+        <v>47</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>43</v>
+      </c>
+      <c r="R25" s="1">
+        <v>118</v>
+      </c>
+      <c r="S25" s="1">
+        <v>129</v>
+      </c>
+      <c r="T25" s="1">
+        <v>185</v>
+      </c>
+      <c r="U25" s="1">
+        <v>157</v>
+      </c>
+      <c r="V25" s="6">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="1">
+        <v>5</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1">
+        <v>7</v>
+      </c>
+      <c r="F26" s="1">
+        <v>36</v>
+      </c>
+      <c r="G26" s="1">
+        <v>71</v>
+      </c>
+      <c r="H26" s="1">
+        <v>35</v>
+      </c>
+      <c r="I26" s="1">
+        <v>46</v>
+      </c>
+      <c r="J26" s="1">
+        <v>66</v>
+      </c>
+      <c r="K26" s="1">
+        <v>103</v>
+      </c>
+      <c r="L26" s="1">
+        <v>167</v>
+      </c>
+      <c r="M26" s="1">
+        <v>430</v>
+      </c>
+      <c r="N26" s="1">
+        <v>76</v>
+      </c>
+      <c r="O26" s="1">
+        <v>80</v>
+      </c>
+      <c r="P26" s="1">
+        <v>47</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>43</v>
+      </c>
+      <c r="R26" s="1">
+        <v>118</v>
+      </c>
+      <c r="S26" s="1">
+        <v>129</v>
+      </c>
+      <c r="T26" s="1">
+        <v>185</v>
+      </c>
+      <c r="U26" s="1">
+        <v>157</v>
+      </c>
+      <c r="V26" s="6">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1">
+        <v>3</v>
+      </c>
+      <c r="E27" s="1">
+        <v>7</v>
+      </c>
+      <c r="F27" s="1">
+        <v>36</v>
+      </c>
+      <c r="G27" s="1">
+        <v>71</v>
+      </c>
+      <c r="H27" s="1">
+        <v>35</v>
+      </c>
+      <c r="I27" s="1">
+        <v>46</v>
+      </c>
+      <c r="J27" s="1">
+        <v>66</v>
+      </c>
+      <c r="K27" s="1">
+        <v>103</v>
+      </c>
+      <c r="L27" s="1">
+        <v>167</v>
+      </c>
+      <c r="M27" s="1">
+        <v>430</v>
+      </c>
+      <c r="N27" s="1">
+        <v>76</v>
+      </c>
+      <c r="O27" s="1">
+        <v>80</v>
+      </c>
+      <c r="P27" s="1">
+        <v>47</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>43</v>
+      </c>
+      <c r="R27" s="1">
+        <v>118</v>
+      </c>
+      <c r="S27" s="1">
+        <v>129</v>
+      </c>
+      <c r="T27" s="1">
+        <v>185</v>
+      </c>
+      <c r="U27" s="1">
+        <v>157</v>
+      </c>
+      <c r="V27" s="6">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="1">
+        <v>10</v>
+      </c>
+      <c r="D28" s="1">
+        <v>19</v>
+      </c>
+      <c r="E28" s="1">
+        <v>33</v>
+      </c>
+      <c r="F28" s="1">
+        <v>126</v>
+      </c>
+      <c r="G28" s="1">
+        <v>668</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1051</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1220</v>
+      </c>
+      <c r="J28" s="1">
+        <v>3096</v>
+      </c>
+      <c r="K28" s="1">
+        <v>2872</v>
+      </c>
+      <c r="L28" s="1">
+        <v>5065</v>
+      </c>
+      <c r="M28" s="1">
+        <v>21437</v>
+      </c>
+      <c r="N28" s="1">
+        <v>18180</v>
+      </c>
+      <c r="O28" s="1">
+        <v>13442</v>
+      </c>
+      <c r="P28" s="1">
+        <v>5397</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>7763</v>
+      </c>
+      <c r="R28" s="1">
+        <v>130088</v>
+      </c>
+      <c r="S28" s="1">
+        <v>152632</v>
+      </c>
+      <c r="T28" s="1">
+        <v>206377</v>
+      </c>
+      <c r="U28" s="1">
+        <v>417153</v>
+      </c>
+      <c r="V28" s="6">
+        <v>797295</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="2">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2">
+        <v>9</v>
+      </c>
+      <c r="F29" s="2">
+        <v>37</v>
+      </c>
+      <c r="G29" s="2">
+        <v>72</v>
+      </c>
+      <c r="H29" s="2">
+        <v>35</v>
+      </c>
+      <c r="I29" s="2">
+        <v>47</v>
+      </c>
+      <c r="J29" s="2">
+        <v>67</v>
+      </c>
+      <c r="K29" s="2">
+        <v>104</v>
+      </c>
+      <c r="L29" s="2">
+        <v>168</v>
+      </c>
+      <c r="M29" s="2">
+        <v>431</v>
+      </c>
+      <c r="N29" s="2">
+        <v>77</v>
+      </c>
+      <c r="O29" s="2">
+        <v>82</v>
+      </c>
+      <c r="P29" s="2">
+        <v>47</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>45</v>
+      </c>
+      <c r="R29" s="2">
+        <v>118</v>
+      </c>
+      <c r="S29" s="2">
+        <v>129</v>
+      </c>
+      <c r="T29" s="2">
+        <v>187</v>
+      </c>
+      <c r="U29" s="2">
+        <v>158</v>
+      </c>
+      <c r="V29" s="8">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="30" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20631,14 +21574,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C2644D-1F5F-4165-B7B9-8E10728AC7F6}">
-  <dimension ref="A1"/>
+  <dimension ref="C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AX68" sqref="AX68"/>
+    <sheetView topLeftCell="A56" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C74" s="10"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
merge of "master" and "origin/master"
</commit_message>
<xml_diff>
--- a/docs/time_analysis.xlsx
+++ b/docs/time_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariana Ramos\Desktop\3ano\iart\IART-g39\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\U. Porto\3 ano\2 semestre\IART-g39\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CB7739-1F6F-4A13-8961-969DA9286052}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98747F34-C6CB-4F5C-B188-360A2241F56D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{80728A2F-030A-4331-A84E-3313CB5F0CBB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{80728A2F-030A-4331-A84E-3313CB5F0CBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Dados" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="39">
   <si>
     <t>Level 1</t>
   </si>
@@ -127,13 +127,31 @@
     <t>Heuristics A*</t>
   </si>
   <si>
-    <t>Heuristic1</t>
+    <t>heuristic1 + depth</t>
   </si>
   <si>
-    <t>Heuristic2</t>
+    <t>heuristic2 + depth</t>
   </si>
   <si>
-    <t>Heuristic3</t>
+    <t>heuristic3 + depth</t>
+  </si>
+  <si>
+    <t>heuristic1</t>
+  </si>
+  <si>
+    <t>heuristic2</t>
+  </si>
+  <si>
+    <t>heuristic3</t>
+  </si>
+  <si>
+    <t>heuristic1 + heuristic2</t>
+  </si>
+  <si>
+    <t>heuristic1 + heuristic3</t>
+  </si>
+  <si>
+    <t>heuristic2 + heuristic3</t>
   </si>
 </sst>
 </file>
@@ -185,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -328,11 +346,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -355,6 +388,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +452,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -526,61 +566,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.011E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9799999999999997E-4</c:v>
+                  <c:v>7.4899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.044E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.4859999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.9710000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.7179999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.6750000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.5469999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0010000000000002E-3</c:v>
+                  <c:v>2.003E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8651000000000001E-2</c:v>
+                  <c:v>2.0733000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.006E-3</c:v>
+                  <c:v>7.3559999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.045E-3</c:v>
+                  <c:v>6.4840000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9970000000000001E-3</c:v>
+                  <c:v>2.0209999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9989999999999999E-3</c:v>
+                  <c:v>1.7669999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.0470000000000003E-3</c:v>
+                  <c:v>6.149E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.9959999999999996E-3</c:v>
+                  <c:v>6.1739999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.0460000000000002E-3</c:v>
+                  <c:v>1.754E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.5869999999999991E-3</c:v>
+                  <c:v>9.7199999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.01</c:v>
+                  <c:v>6.8019999999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -645,7 +685,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="754962064"/>
@@ -727,7 +767,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -759,7 +799,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="754961744"/>
@@ -807,7 +847,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -888,7 +928,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1002,61 +1042,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.011E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9799999999999997E-4</c:v>
+                  <c:v>7.4899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.044E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.4859999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.9710000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.7179999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.6750000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.5469999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0010000000000002E-3</c:v>
+                  <c:v>2.003E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8651000000000001E-2</c:v>
+                  <c:v>2.0733000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.006E-3</c:v>
+                  <c:v>7.3559999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.045E-3</c:v>
+                  <c:v>6.4840000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9970000000000001E-3</c:v>
+                  <c:v>2.0209999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9989999999999999E-3</c:v>
+                  <c:v>1.7669999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.0470000000000003E-3</c:v>
+                  <c:v>6.149E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.9959999999999996E-3</c:v>
+                  <c:v>6.1739999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.0460000000000002E-3</c:v>
+                  <c:v>1.754E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.5869999999999991E-3</c:v>
+                  <c:v>9.7199999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.01</c:v>
+                  <c:v>6.8019999999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2035,7 +2075,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488930568"/>
@@ -2122,7 +2162,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2154,7 +2194,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488930248"/>
@@ -2196,7 +2236,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2233,7 +2273,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2314,7 +2354,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2428,61 +2468,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.011E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9799999999999997E-4</c:v>
+                  <c:v>7.4899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.044E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.4859999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.9710000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.7179999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.6750000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.5469999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0010000000000002E-3</c:v>
+                  <c:v>2.003E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8651000000000001E-2</c:v>
+                  <c:v>2.0733000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.006E-3</c:v>
+                  <c:v>7.3559999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.045E-3</c:v>
+                  <c:v>6.4840000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9970000000000001E-3</c:v>
+                  <c:v>2.0209999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9989999999999999E-3</c:v>
+                  <c:v>1.7669999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.0470000000000003E-3</c:v>
+                  <c:v>6.149E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.9959999999999996E-3</c:v>
+                  <c:v>6.1739999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.0460000000000002E-3</c:v>
+                  <c:v>1.754E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.5869999999999991E-3</c:v>
+                  <c:v>9.7199999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.01</c:v>
+                  <c:v>6.8019999999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3481,7 +3521,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488915848"/>
@@ -3563,7 +3603,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3595,7 +3635,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="488912328"/>
@@ -3637,7 +3677,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3674,7 +3714,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3755,7 +3795,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4158,7 +4198,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="576048336"/>
@@ -4240,7 +4280,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4272,7 +4312,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="576045136"/>
@@ -4314,7 +4354,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4351,7 +4391,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4427,7 +4467,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4541,61 +4581,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.011E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9799999999999997E-4</c:v>
+                  <c:v>7.4899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.044E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.4859999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.9710000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.7179999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.6750000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.5469999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0010000000000002E-3</c:v>
+                  <c:v>2.003E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8651000000000001E-2</c:v>
+                  <c:v>2.0733000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.006E-3</c:v>
+                  <c:v>7.3559999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.045E-3</c:v>
+                  <c:v>6.4840000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9970000000000001E-3</c:v>
+                  <c:v>2.0209999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9989999999999999E-3</c:v>
+                  <c:v>1.7669999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.0470000000000003E-3</c:v>
+                  <c:v>6.149E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.9959999999999996E-3</c:v>
+                  <c:v>6.1739999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.0460000000000002E-3</c:v>
+                  <c:v>1.754E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.5869999999999991E-3</c:v>
+                  <c:v>9.7199999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.01</c:v>
+                  <c:v>6.8019999999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5170,7 +5210,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="576048336"/>
@@ -5252,7 +5292,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5284,7 +5324,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="576045136"/>
@@ -5330,7 +5370,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5367,7 +5407,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5448,7 +5488,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6361,7 +6401,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="538156144"/>
@@ -6418,7 +6458,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6450,7 +6490,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="538157128"/>
@@ -6493,7 +6533,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6530,7 +6570,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6611,7 +6651,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6626,11 +6666,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dados!$B$33</c:f>
+              <c:f>Dados!$B$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Heuristic1</c:v>
+                  <c:v>heuristic1 + depth</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6717,7 +6757,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Dados!$C$33:$V$33</c:f>
+              <c:f>Dados!$C$36:$V$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -6725,61 +6765,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.011E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9799999999999997E-4</c:v>
+                  <c:v>7.4899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.044E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.4859999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.9710000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.7179999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.6750000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.5469999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0010000000000002E-3</c:v>
+                  <c:v>2.003E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8651000000000001E-2</c:v>
+                  <c:v>2.0733000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.006E-3</c:v>
+                  <c:v>7.3559999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.045E-3</c:v>
+                  <c:v>6.4840000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9970000000000001E-3</c:v>
+                  <c:v>2.0209999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9989999999999999E-3</c:v>
+                  <c:v>1.7669999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.0470000000000003E-3</c:v>
+                  <c:v>6.149E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.9959999999999996E-3</c:v>
+                  <c:v>6.1739999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.0460000000000002E-3</c:v>
+                  <c:v>1.754E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.5869999999999991E-3</c:v>
+                  <c:v>9.7199999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.01</c:v>
+                  <c:v>6.8019999999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6796,11 +6836,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dados!$B$34</c:f>
+              <c:f>Dados!$B$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Heuristic2</c:v>
+                  <c:v>heuristic2 + depth</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6887,69 +6927,69 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Dados!$C$34:$V$34</c:f>
+              <c:f>Dados!$C$37:$V$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1E-3</c:v>
+                  <c:v>7.3099999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9799999999999997E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5600000000000004E-4</c:v>
+                  <c:v>1.0369999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.238E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0010000000000002E-3</c:v>
+                  <c:v>1.374E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.003E-3</c:v>
+                  <c:v>3.555E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9970000000000001E-3</c:v>
+                  <c:v>1.7279999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>4.4990000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3739999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.953E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6542999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.065E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.7070000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1.0020000000000001E-3</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.003E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7.0029999999999997E-3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.583E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2.9989999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.0010000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.0010000000000002E-3</c:v>
-                </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0039999999999999E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.999E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.0992999999999999E-2</c:v>
+                  <c:v>8.8970000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.9989999999999992E-3</c:v>
+                  <c:v>9.2680000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.0998000000000001E-2</c:v>
+                  <c:v>1.8393E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.6089999999999995E-3</c:v>
+                  <c:v>1.5407000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6966,11 +7006,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Dados!$B$35</c:f>
+              <c:f>Dados!$B$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Heuristic3</c:v>
+                  <c:v>heuristic3 + depth</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7057,69 +7097,69 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Dados!$C$35:$V$35</c:f>
+              <c:f>Dados!$C$38:$V$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>9.9599999999999992E-4</c:v>
+                  <c:v>1.044E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2.4000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1E-3</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.0449999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9969999999999997E-3</c:v>
+                  <c:v>4.071E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9970000000000001E-3</c:v>
+                  <c:v>1.2179999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9989999999999999E-3</c:v>
+                  <c:v>1.6720000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.9960000000000004E-3</c:v>
+                  <c:v>1.3290000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9970000000000001E-3</c:v>
+                  <c:v>1.97E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9950000000000003E-3</c:v>
+                  <c:v>2.96E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.5025999999999999E-2</c:v>
+                  <c:v>1.6677999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.0070000000000001E-3</c:v>
+                  <c:v>3.735E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>1.008E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.9949999999999998E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9989999999999999E-3</c:v>
+                  <c:v>4.6909999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.0359999999999997E-3</c:v>
+                  <c:v>1.3799999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.9949999999999995E-3</c:v>
+                  <c:v>8.8120000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.5502E-2</c:v>
+                  <c:v>7.0660000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.9589999999999999E-3</c:v>
+                  <c:v>4.6470000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.3762E-2</c:v>
+                  <c:v>8.0219999999999996E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7184,7 +7224,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="536035248"/>
@@ -7266,7 +7306,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7298,7 +7338,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="536032296"/>
@@ -7340,7 +7380,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -7370,7 +7410,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7421,7 +7461,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7737,61 +7777,61 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.011E-3</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>9.9799999999999997E-4</c:v>
+                        <c:v>7.4899999999999999E-4</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1E-3</c:v>
+                        <c:v>1.044E-3</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.4859999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1E-3</c:v>
+                        <c:v>1.9710000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.7179999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.6750000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>2E-3</c:v>
+                        <c:v>3.5469999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>4.0010000000000002E-3</c:v>
+                        <c:v>2.003E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>1.8651000000000001E-2</c:v>
+                        <c:v>2.0733000000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>2.006E-3</c:v>
+                        <c:v>7.3559999999999997E-3</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>3.045E-3</c:v>
+                        <c:v>6.4840000000000002E-3</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>1.9970000000000001E-3</c:v>
+                        <c:v>2.0209999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>1.9989999999999999E-3</c:v>
+                        <c:v>1.7669999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>5.0470000000000003E-3</c:v>
+                        <c:v>6.149E-3</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>6.9959999999999996E-3</c:v>
+                        <c:v>6.1739999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>7.0460000000000002E-3</c:v>
+                        <c:v>1.754E-2</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>8.5869999999999991E-3</c:v>
+                        <c:v>9.7199999999999995E-3</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>0.01</c:v>
+                        <c:v>6.8019999999999999E-3</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -7848,7 +7888,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="756610000"/>
@@ -7930,7 +7970,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -7962,7 +8002,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="756609680"/>
@@ -8010,7 +8050,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8091,7 +8131,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -8205,61 +8245,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.011E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9799999999999997E-4</c:v>
+                  <c:v>7.4899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.044E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.4859999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.9710000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.7179999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.6750000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.5469999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0010000000000002E-3</c:v>
+                  <c:v>2.003E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8651000000000001E-2</c:v>
+                  <c:v>2.0733000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.006E-3</c:v>
+                  <c:v>7.3559999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.045E-3</c:v>
+                  <c:v>6.4840000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9970000000000001E-3</c:v>
+                  <c:v>2.0209999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9989999999999999E-3</c:v>
+                  <c:v>1.7669999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.0470000000000003E-3</c:v>
+                  <c:v>6.149E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.9959999999999996E-3</c:v>
+                  <c:v>6.1739999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.0460000000000002E-3</c:v>
+                  <c:v>1.754E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.5869999999999991E-3</c:v>
+                  <c:v>9.7199999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.01</c:v>
+                  <c:v>6.8019999999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9004,7 +9044,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="576048336"/>
@@ -9086,7 +9126,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -9118,7 +9158,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="576045136"/>
@@ -9160,7 +9200,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -9197,7 +9237,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9248,7 +9288,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -9564,61 +9604,61 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.011E-3</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>9.9799999999999997E-4</c:v>
+                        <c:v>7.4899999999999999E-4</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1E-3</c:v>
+                        <c:v>1.044E-3</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.4859999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1E-3</c:v>
+                        <c:v>1.9710000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.7179999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.6750000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>2E-3</c:v>
+                        <c:v>3.5469999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>4.0010000000000002E-3</c:v>
+                        <c:v>2.003E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>1.8651000000000001E-2</c:v>
+                        <c:v>2.0733000000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>2.006E-3</c:v>
+                        <c:v>7.3559999999999997E-3</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>3.045E-3</c:v>
+                        <c:v>6.4840000000000002E-3</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>1.9970000000000001E-3</c:v>
+                        <c:v>2.0209999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>1.9989999999999999E-3</c:v>
+                        <c:v>1.7669999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>5.0470000000000003E-3</c:v>
+                        <c:v>6.149E-3</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>6.9959999999999996E-3</c:v>
+                        <c:v>6.1739999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>7.0460000000000002E-3</c:v>
+                        <c:v>1.754E-2</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>8.5869999999999991E-3</c:v>
+                        <c:v>9.7199999999999995E-3</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>0.01</c:v>
+                        <c:v>6.8019999999999999E-3</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -10245,7 +10285,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="537058168"/>
@@ -10336,7 +10376,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -10368,7 +10408,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="511954160"/>
@@ -10416,7 +10456,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10467,7 +10507,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -10783,61 +10823,61 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.011E-3</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>9.9799999999999997E-4</c:v>
+                        <c:v>7.4899999999999999E-4</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1E-3</c:v>
+                        <c:v>1.044E-3</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.4859999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1E-3</c:v>
+                        <c:v>1.9710000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.7179999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.6750000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>2E-3</c:v>
+                        <c:v>3.5469999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>4.0010000000000002E-3</c:v>
+                        <c:v>2.003E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>1.8651000000000001E-2</c:v>
+                        <c:v>2.0733000000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>2.006E-3</c:v>
+                        <c:v>7.3559999999999997E-3</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>3.045E-3</c:v>
+                        <c:v>6.4840000000000002E-3</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>1.9970000000000001E-3</c:v>
+                        <c:v>2.0209999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>1.9989999999999999E-3</c:v>
+                        <c:v>1.7669999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>5.0470000000000003E-3</c:v>
+                        <c:v>6.149E-3</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>6.9959999999999996E-3</c:v>
+                        <c:v>6.1739999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>7.0460000000000002E-3</c:v>
+                        <c:v>1.754E-2</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>8.5869999999999991E-3</c:v>
+                        <c:v>9.7199999999999995E-3</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>0.01</c:v>
+                        <c:v>6.8019999999999999E-3</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -11464,7 +11504,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="584061048"/>
@@ -11555,7 +11595,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -11587,7 +11627,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="584063608"/>
@@ -11635,7 +11675,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -11686,7 +11726,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -12002,61 +12042,61 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.011E-3</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>9.9799999999999997E-4</c:v>
+                        <c:v>7.4899999999999999E-4</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1E-3</c:v>
+                        <c:v>1.044E-3</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.4859999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1E-3</c:v>
+                        <c:v>1.9710000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.7179999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.6750000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>2E-3</c:v>
+                        <c:v>3.5469999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>4.0010000000000002E-3</c:v>
+                        <c:v>2.003E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>1.8651000000000001E-2</c:v>
+                        <c:v>2.0733000000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>2.006E-3</c:v>
+                        <c:v>7.3559999999999997E-3</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>3.045E-3</c:v>
+                        <c:v>6.4840000000000002E-3</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>1.9970000000000001E-3</c:v>
+                        <c:v>2.0209999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>1.9989999999999999E-3</c:v>
+                        <c:v>1.7669999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>5.0470000000000003E-3</c:v>
+                        <c:v>6.149E-3</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>6.9959999999999996E-3</c:v>
+                        <c:v>6.1739999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>7.0460000000000002E-3</c:v>
+                        <c:v>1.754E-2</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>8.5869999999999991E-3</c:v>
+                        <c:v>9.7199999999999995E-3</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>0.01</c:v>
+                        <c:v>6.8019999999999999E-3</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -12683,7 +12723,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="584124728"/>
@@ -12774,7 +12814,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -12806,7 +12846,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="576075856"/>
@@ -12854,7 +12894,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -12935,7 +12975,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -13421,61 +13461,61 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.011E-3</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>9.9799999999999997E-4</c:v>
+                        <c:v>7.4899999999999999E-4</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1E-3</c:v>
+                        <c:v>1.044E-3</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.4859999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1E-3</c:v>
+                        <c:v>1.9710000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.7179999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.6750000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>2E-3</c:v>
+                        <c:v>3.5469999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>4.0010000000000002E-3</c:v>
+                        <c:v>2.003E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>1.8651000000000001E-2</c:v>
+                        <c:v>2.0733000000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>2.006E-3</c:v>
+                        <c:v>7.3559999999999997E-3</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>3.045E-3</c:v>
+                        <c:v>6.4840000000000002E-3</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>1.9970000000000001E-3</c:v>
+                        <c:v>2.0209999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>1.9989999999999999E-3</c:v>
+                        <c:v>1.7669999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>5.0470000000000003E-3</c:v>
+                        <c:v>6.149E-3</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>6.9959999999999996E-3</c:v>
+                        <c:v>6.1739999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>7.0460000000000002E-3</c:v>
+                        <c:v>1.754E-2</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>8.5869999999999991E-3</c:v>
+                        <c:v>9.7199999999999995E-3</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>0.01</c:v>
+                        <c:v>6.8019999999999999E-3</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -14102,7 +14142,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="530106040"/>
@@ -14189,7 +14229,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -14221,7 +14261,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="530105080"/>
@@ -14263,7 +14303,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -14300,7 +14340,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -14385,7 +14425,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -14499,61 +14539,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.011E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9799999999999997E-4</c:v>
+                  <c:v>7.4899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.044E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.4859999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>1.9710000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.7179999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2E-3</c:v>
+                  <c:v>1.6750000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2E-3</c:v>
+                  <c:v>3.5469999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0010000000000002E-3</c:v>
+                  <c:v>2.003E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.8651000000000001E-2</c:v>
+                  <c:v>2.0733000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.006E-3</c:v>
+                  <c:v>7.3559999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.045E-3</c:v>
+                  <c:v>6.4840000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9970000000000001E-3</c:v>
+                  <c:v>2.0209999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9989999999999999E-3</c:v>
+                  <c:v>1.7669999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.0470000000000003E-3</c:v>
+                  <c:v>6.149E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.9959999999999996E-3</c:v>
+                  <c:v>6.1739999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.0460000000000002E-3</c:v>
+                  <c:v>1.754E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.5869999999999991E-3</c:v>
+                  <c:v>9.7199999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.01</c:v>
+                  <c:v>6.8019999999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15492,7 +15532,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="576068816"/>
@@ -15574,7 +15614,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -15606,7 +15646,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="576068176"/>
@@ -15649,7 +15689,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -15686,7 +15726,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -15737,7 +15777,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -16053,61 +16093,61 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.011E-3</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>9.9799999999999997E-4</c:v>
+                        <c:v>7.4899999999999999E-4</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1E-3</c:v>
+                        <c:v>1.044E-3</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.4859999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1E-3</c:v>
+                        <c:v>1.9710000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.7179999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>2E-3</c:v>
+                        <c:v>1.6750000000000001E-3</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>2E-3</c:v>
+                        <c:v>3.5469999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>4.0010000000000002E-3</c:v>
+                        <c:v>2.003E-3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>1.8651000000000001E-2</c:v>
+                        <c:v>2.0733000000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>2.006E-3</c:v>
+                        <c:v>7.3559999999999997E-3</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>3.045E-3</c:v>
+                        <c:v>6.4840000000000002E-3</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>1.9970000000000001E-3</c:v>
+                        <c:v>2.0209999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>1.9989999999999999E-3</c:v>
+                        <c:v>1.7669999999999999E-3</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>5.0470000000000003E-3</c:v>
+                        <c:v>6.149E-3</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>6.9959999999999996E-3</c:v>
+                        <c:v>6.1739999999999998E-3</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>7.0460000000000002E-3</c:v>
+                        <c:v>1.754E-2</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>8.5869999999999991E-3</c:v>
+                        <c:v>9.7199999999999995E-3</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>0.01</c:v>
+                        <c:v>6.8019999999999999E-3</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -16924,7 +16964,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="537671288"/>
@@ -17011,7 +17051,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -17043,7 +17083,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="537671928"/>
@@ -17091,7 +17131,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -26292,19 +26332,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8F887B-5E63-41C2-AD6C-350EA53EFBC0}">
-  <dimension ref="B2:V35"/>
+  <dimension ref="B2:V42"/>
   <sheetViews>
-    <sheetView topLeftCell="D26" zoomScale="53" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R56" sqref="R56"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="22" width="16.7109375" customWidth="1"/>
+    <col min="2" max="22" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
         <v>26</v>
       </c>
@@ -26369,72 +26409,72 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" s="1">
-        <v>1.011E-3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>9.9799999999999997E-4</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2E-3</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="I4" s="1">
-        <v>2E-3</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2E-3</v>
-      </c>
-      <c r="K4" s="1">
-        <v>2E-3</v>
-      </c>
-      <c r="L4" s="1">
-        <v>4.0010000000000002E-3</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1.8651000000000001E-2</v>
-      </c>
-      <c r="N4" s="1">
-        <v>2.006E-3</v>
-      </c>
-      <c r="O4" s="1">
-        <v>3.045E-3</v>
-      </c>
-      <c r="P4" s="1">
-        <v>1.9970000000000001E-3</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>1.9989999999999999E-3</v>
-      </c>
-      <c r="R4" s="1">
-        <v>5.0470000000000003E-3</v>
-      </c>
-      <c r="S4" s="1">
-        <v>6.9959999999999996E-3</v>
-      </c>
-      <c r="T4" s="1">
-        <v>7.0460000000000002E-3</v>
-      </c>
-      <c r="U4" s="1">
-        <v>8.5869999999999991E-3</v>
-      </c>
-      <c r="V4" s="6">
-        <v>0.01</v>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>7.4899999999999999E-4</v>
+      </c>
+      <c r="F4">
+        <v>1.044E-3</v>
+      </c>
+      <c r="G4">
+        <v>1.4859999999999999E-3</v>
+      </c>
+      <c r="H4">
+        <v>1.9710000000000001E-3</v>
+      </c>
+      <c r="I4">
+        <v>1.7179999999999999E-3</v>
+      </c>
+      <c r="J4">
+        <v>1.6750000000000001E-3</v>
+      </c>
+      <c r="K4">
+        <v>3.5469999999999998E-3</v>
+      </c>
+      <c r="L4">
+        <v>2.003E-3</v>
+      </c>
+      <c r="M4">
+        <v>2.0733000000000001E-2</v>
+      </c>
+      <c r="N4">
+        <v>7.3559999999999997E-3</v>
+      </c>
+      <c r="O4">
+        <v>6.4840000000000002E-3</v>
+      </c>
+      <c r="P4">
+        <v>2.0209999999999998E-3</v>
+      </c>
+      <c r="Q4">
+        <v>1.7669999999999999E-3</v>
+      </c>
+      <c r="R4">
+        <v>6.149E-3</v>
+      </c>
+      <c r="S4">
+        <v>6.1739999999999998E-3</v>
+      </c>
+      <c r="T4">
+        <v>1.754E-2</v>
+      </c>
+      <c r="U4">
+        <v>9.7199999999999995E-3</v>
+      </c>
+      <c r="V4">
+        <v>6.8019999999999999E-3</v>
       </c>
     </row>
-    <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
@@ -26499,7 +26539,7 @@
         <v>1.5731999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
@@ -26564,7 +26604,7 @@
         <v>1.7003000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>24</v>
       </c>
@@ -26629,7 +26669,7 @@
         <v>6.1940000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
@@ -26694,7 +26734,7 @@
         <v>111.457792</v>
       </c>
     </row>
-    <row r="9" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
@@ -26759,9 +26799,9 @@
         <v>1.6997000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="9" t="s">
         <v>27</v>
       </c>
@@ -26826,7 +26866,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
@@ -26891,7 +26931,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
@@ -26956,7 +26996,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
@@ -27021,7 +27061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
@@ -27086,7 +27126,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
         <v>25</v>
       </c>
@@ -27099,7 +27139,7 @@
       <c r="E18" s="1">
         <v>3</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="11">
         <v>4</v>
       </c>
       <c r="G18" s="1">
@@ -27151,7 +27191,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7" t="s">
         <v>20</v>
       </c>
@@ -27216,9 +27256,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="2:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="9" t="s">
         <v>28</v>
       </c>
@@ -27283,7 +27323,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
@@ -27348,7 +27388,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
         <v>21</v>
       </c>
@@ -27413,7 +27453,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
@@ -27478,7 +27518,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
@@ -27543,7 +27583,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="28" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
@@ -27608,7 +27648,7 @@
         <v>797295</v>
       </c>
     </row>
-    <row r="29" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="7" t="s">
         <v>20</v>
       </c>
@@ -27630,7 +27670,7 @@
       <c r="H29" s="2">
         <v>35</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="14">
         <v>47</v>
       </c>
       <c r="J29" s="2">
@@ -27673,9 +27713,9 @@
         <v>204</v>
       </c>
     </row>
-    <row r="30" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="2:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="2:22" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="9" t="s">
         <v>29</v>
       </c>
@@ -27740,200 +27780,593 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2.5699999999999998E-3</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1.047E-3</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>2.944E-3</v>
+      </c>
+      <c r="G33" s="1">
+        <v>4.0679999999999996E-3</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1.8469999999999999E-3</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1">
+        <v>9.3150000000000004E-3</v>
+      </c>
+      <c r="L33" s="1">
+        <v>5.2579999999999997E-3</v>
+      </c>
+      <c r="M33" s="1">
+        <v>8.6169999999999997E-3</v>
+      </c>
+      <c r="N33" s="1">
+        <v>1.041E-3</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1">
+        <v>7.9399999999999991E-3</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>1.7060000000000001E-3</v>
+      </c>
+      <c r="R33" s="1">
+        <v>1.5640000000000001E-3</v>
+      </c>
+      <c r="S33" s="1">
+        <v>0</v>
+      </c>
+      <c r="T33" s="1">
+        <v>1.155E-2</v>
+      </c>
+      <c r="U33" s="1">
+        <v>7.9959999999999996E-3</v>
+      </c>
+      <c r="V33" s="6">
+        <v>1.0673E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3.0400000000000002E-4</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1.039E-3</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1.4419999999999999E-3</v>
+      </c>
+      <c r="G34" s="1">
+        <v>5.5110000000000003E-3</v>
+      </c>
+      <c r="H34" s="1">
+        <v>2.774E-3</v>
+      </c>
+      <c r="I34" s="1">
+        <v>3.284E-3</v>
+      </c>
+      <c r="J34" s="1">
+        <v>1.039E-3</v>
+      </c>
+      <c r="K34" s="1">
+        <v>2.042E-3</v>
+      </c>
+      <c r="L34" s="1">
+        <v>1.2897E-2</v>
+      </c>
+      <c r="M34" s="1">
+        <v>4.8190000000000004E-3</v>
+      </c>
+      <c r="N34" s="1">
+        <v>6.5909999999999996E-3</v>
+      </c>
+      <c r="O34" s="1">
+        <v>3.3649999999999999E-3</v>
+      </c>
+      <c r="P34" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>1.9810000000000001E-3</v>
+      </c>
+      <c r="R34" s="1">
+        <v>1.9980000000000002E-3</v>
+      </c>
+      <c r="S34" s="1">
+        <v>7.6660000000000001E-3</v>
+      </c>
+      <c r="T34" s="1">
+        <v>6.8300000000000001E-3</v>
+      </c>
+      <c r="U34" s="1">
+        <v>8.2950000000000003E-3</v>
+      </c>
+      <c r="V34" s="6">
+        <v>1.6258000000000002E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1.0449999999999999E-3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>3.19E-4</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1.0449999999999999E-3</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1.9610000000000001E-3</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1">
+        <v>4.4050000000000001E-3</v>
+      </c>
+      <c r="K35" s="1">
+        <v>3.2320000000000001E-3</v>
+      </c>
+      <c r="L35" s="1">
+        <v>0</v>
+      </c>
+      <c r="M35" s="1">
+        <v>9.3109999999999998E-3</v>
+      </c>
+      <c r="N35" s="1">
+        <v>9.1020000000000007E-3</v>
+      </c>
+      <c r="O35" s="1">
+        <v>2.3679999999999999E-3</v>
+      </c>
+      <c r="P35" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>6.1520000000000004E-3</v>
+      </c>
+      <c r="R35" s="1">
+        <v>1.905E-3</v>
+      </c>
+      <c r="S35" s="1">
+        <v>4.5500000000000002E-3</v>
+      </c>
+      <c r="T35" s="1">
+        <v>1.1573999999999999E-2</v>
+      </c>
+      <c r="U35" s="1">
+        <v>4.1669999999999997E-3</v>
+      </c>
+      <c r="V35" s="6">
+        <v>1.044E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C36" s="1">
         <v>0</v>
       </c>
-      <c r="D33" s="1">
-        <v>1.011E-3</v>
-      </c>
-      <c r="E33" s="1">
-        <v>9.9799999999999997E-4</v>
-      </c>
-      <c r="F33" s="1">
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>7.4899999999999999E-4</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1.044E-3</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1.4859999999999999E-3</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1.9710000000000001E-3</v>
+      </c>
+      <c r="I36" s="1">
+        <v>1.7179999999999999E-3</v>
+      </c>
+      <c r="J36" s="1">
+        <v>1.6750000000000001E-3</v>
+      </c>
+      <c r="K36" s="1">
+        <v>3.5469999999999998E-3</v>
+      </c>
+      <c r="L36" s="1">
+        <v>2.003E-3</v>
+      </c>
+      <c r="M36" s="1">
+        <v>2.0733000000000001E-2</v>
+      </c>
+      <c r="N36" s="1">
+        <v>7.3559999999999997E-3</v>
+      </c>
+      <c r="O36" s="1">
+        <v>6.4840000000000002E-3</v>
+      </c>
+      <c r="P36" s="1">
+        <v>2.0209999999999998E-3</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>1.7669999999999999E-3</v>
+      </c>
+      <c r="R36" s="1">
+        <v>6.149E-3</v>
+      </c>
+      <c r="S36" s="1">
+        <v>6.1739999999999998E-3</v>
+      </c>
+      <c r="T36" s="1">
+        <v>1.754E-2</v>
+      </c>
+      <c r="U36" s="1">
+        <v>9.7199999999999995E-3</v>
+      </c>
+      <c r="V36" s="6">
+        <v>6.8019999999999999E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="1">
+        <v>7.3099999999999999E-4</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1.0369999999999999E-3</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1.238E-3</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1.374E-3</v>
+      </c>
+      <c r="H37" s="1">
+        <v>3.555E-3</v>
+      </c>
+      <c r="I37" s="1">
+        <v>1.7279999999999999E-3</v>
+      </c>
+      <c r="J37" s="1">
+        <v>4.4990000000000004E-3</v>
+      </c>
+      <c r="K37" s="1">
+        <v>3.3739999999999998E-3</v>
+      </c>
+      <c r="L37" s="1">
+        <v>6.953E-3</v>
+      </c>
+      <c r="M37" s="1">
+        <v>1.6542999999999999E-2</v>
+      </c>
+      <c r="N37" s="1">
+        <v>3.065E-3</v>
+      </c>
+      <c r="O37" s="1">
+        <v>2.7070000000000002E-3</v>
+      </c>
+      <c r="P37" s="1">
+        <v>1.0020000000000001E-3</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0</v>
+      </c>
+      <c r="R37" s="1">
+        <v>0</v>
+      </c>
+      <c r="S37" s="1">
+        <v>8.8970000000000004E-3</v>
+      </c>
+      <c r="T37" s="1">
+        <v>9.2680000000000002E-3</v>
+      </c>
+      <c r="U37" s="1">
+        <v>1.8393E-2</v>
+      </c>
+      <c r="V37" s="6">
+        <v>1.5407000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1.044E-3</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1.0449999999999999E-3</v>
+      </c>
+      <c r="G38" s="1">
+        <v>4.071E-3</v>
+      </c>
+      <c r="H38" s="1">
+        <v>1.2179999999999999E-3</v>
+      </c>
+      <c r="I38" s="1">
+        <v>1.6720000000000001E-3</v>
+      </c>
+      <c r="J38" s="1">
+        <v>1.3290000000000001E-3</v>
+      </c>
+      <c r="K38" s="1">
+        <v>1.97E-3</v>
+      </c>
+      <c r="L38" s="1">
+        <v>2.96E-3</v>
+      </c>
+      <c r="M38" s="1">
+        <v>1.6677999999999998E-2</v>
+      </c>
+      <c r="N38" s="1">
+        <v>3.735E-3</v>
+      </c>
+      <c r="O38" s="1">
+        <v>1.008E-3</v>
+      </c>
+      <c r="P38" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>4.6909999999999999E-3</v>
+      </c>
+      <c r="R38" s="1">
+        <v>1.3799999999999999E-3</v>
+      </c>
+      <c r="S38" s="1">
+        <v>8.8120000000000004E-3</v>
+      </c>
+      <c r="T38" s="1">
+        <v>7.0660000000000002E-3</v>
+      </c>
+      <c r="U38" s="1">
+        <v>4.6470000000000001E-3</v>
+      </c>
+      <c r="V38" s="6">
+        <v>8.0219999999999996E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1.042E-3</v>
+      </c>
+      <c r="F39" s="1">
         <v>1E-3</v>
       </c>
-      <c r="G33" s="1">
-        <v>2E-3</v>
-      </c>
-      <c r="H33" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="I33" s="1">
-        <v>2E-3</v>
-      </c>
-      <c r="J33" s="1">
-        <v>2E-3</v>
-      </c>
-      <c r="K33" s="1">
-        <v>2E-3</v>
-      </c>
-      <c r="L33" s="1">
-        <v>4.0010000000000002E-3</v>
-      </c>
-      <c r="M33" s="1">
-        <v>1.8651000000000001E-2</v>
-      </c>
-      <c r="N33" s="1">
-        <v>2.006E-3</v>
-      </c>
-      <c r="O33" s="1">
-        <v>3.045E-3</v>
-      </c>
-      <c r="P33" s="1">
-        <v>1.9970000000000001E-3</v>
-      </c>
-      <c r="Q33" s="1">
-        <v>1.9989999999999999E-3</v>
-      </c>
-      <c r="R33" s="1">
-        <v>5.0470000000000003E-3</v>
-      </c>
-      <c r="S33" s="1">
-        <v>6.9959999999999996E-3</v>
-      </c>
-      <c r="T33" s="1">
-        <v>7.0460000000000002E-3</v>
-      </c>
-      <c r="U33" s="1">
-        <v>8.5869999999999991E-3</v>
-      </c>
-      <c r="V33" s="6">
-        <v>0.01</v>
+      <c r="G39" s="1">
+        <v>2.7269999999999998E-3</v>
+      </c>
+      <c r="H39" s="1">
+        <v>2.1649999999999998E-3</v>
+      </c>
+      <c r="I39" s="1">
+        <v>1.676E-3</v>
+      </c>
+      <c r="J39" s="1">
+        <v>1.6770000000000001E-3</v>
+      </c>
+      <c r="K39" s="1">
+        <v>2.4610000000000001E-3</v>
+      </c>
+      <c r="L39" s="1">
+        <v>0</v>
+      </c>
+      <c r="M39" s="1">
+        <v>8.5330000000000007E-3</v>
+      </c>
+      <c r="N39" s="1">
+        <v>0</v>
+      </c>
+      <c r="O39" s="1">
+        <v>8.208E-3</v>
+      </c>
+      <c r="P39" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>4.9360000000000003E-3</v>
+      </c>
+      <c r="R39" s="1">
+        <v>1.5349999999999999E-3</v>
+      </c>
+      <c r="S39" s="1">
+        <v>3.0309999999999998E-3</v>
+      </c>
+      <c r="T39" s="1">
+        <v>6.8570000000000002E-3</v>
+      </c>
+      <c r="U39" s="1">
+        <v>8.2249999999999997E-3</v>
+      </c>
+      <c r="V39" s="6">
+        <v>9.1009999999999997E-3</v>
       </c>
     </row>
-    <row r="34" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="D34" s="1">
-        <v>9.9799999999999997E-4</v>
-      </c>
-      <c r="E34" s="1">
-        <v>9.5600000000000004E-4</v>
-      </c>
-      <c r="F34" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="G34" s="1">
-        <v>2.0010000000000002E-3</v>
-      </c>
-      <c r="H34" s="1">
-        <v>2.003E-3</v>
-      </c>
-      <c r="I34" s="1">
-        <v>1.9970000000000001E-3</v>
-      </c>
-      <c r="J34" s="1">
-        <v>1.0020000000000001E-3</v>
-      </c>
-      <c r="K34" s="1">
-        <v>3.003E-3</v>
-      </c>
-      <c r="L34" s="1">
-        <v>7.0029999999999997E-3</v>
-      </c>
-      <c r="M34" s="1">
-        <v>1.583E-2</v>
-      </c>
-      <c r="N34" s="1">
-        <v>2.9989999999999999E-3</v>
-      </c>
-      <c r="O34" s="1">
-        <v>3.0010000000000002E-3</v>
-      </c>
-      <c r="P34" s="1">
-        <v>2.0010000000000002E-3</v>
-      </c>
-      <c r="Q34" s="1">
-        <v>1.0039999999999999E-3</v>
-      </c>
-      <c r="R34" s="1">
-        <v>3.999E-3</v>
-      </c>
-      <c r="S34" s="1">
-        <v>1.0992999999999999E-2</v>
-      </c>
-      <c r="T34" s="1">
-        <v>7.9989999999999992E-3</v>
-      </c>
-      <c r="U34" s="1">
-        <v>1.0998000000000001E-2</v>
-      </c>
-      <c r="V34" s="6">
-        <v>9.6089999999999995E-3</v>
+    <row r="40" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>2.0230000000000001E-3</v>
+      </c>
+      <c r="F40" s="1">
+        <v>5.6610000000000002E-3</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1.4371999999999999E-2</v>
+      </c>
+      <c r="H40" s="1">
+        <v>7.4229999999999999E-3</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0</v>
+      </c>
+      <c r="K40" s="1">
+        <v>8.1960000000000002E-3</v>
+      </c>
+      <c r="L40" s="1">
+        <v>7.5170000000000002E-3</v>
+      </c>
+      <c r="M40" s="1">
+        <v>1.4852000000000001E-2</v>
+      </c>
+      <c r="N40" s="1">
+        <v>1.4565E-2</v>
+      </c>
+      <c r="O40" s="1">
+        <v>8.6960000000000006E-3</v>
+      </c>
+      <c r="P40" s="1">
+        <v>2.643E-3</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>2.9729999999999999E-3</v>
+      </c>
+      <c r="R40" s="1">
+        <v>1.851E-3</v>
+      </c>
+      <c r="S40" s="1">
+        <v>1.4186000000000001E-2</v>
+      </c>
+      <c r="T40" s="1">
+        <v>1.4963000000000001E-2</v>
+      </c>
+      <c r="U40" s="1">
+        <v>1.4354E-2</v>
+      </c>
+      <c r="V40" s="6">
+        <v>6.0829999999999999E-3</v>
       </c>
     </row>
-    <row r="35" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="1">
-        <v>9.9599999999999992E-4</v>
-      </c>
-      <c r="D35" s="1">
+    <row r="41" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="2">
+        <v>3.48E-4</v>
+      </c>
+      <c r="D41" s="2">
         <v>0</v>
       </c>
-      <c r="E35" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="F35" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="G35" s="1">
-        <v>4.9969999999999997E-3</v>
-      </c>
-      <c r="H35" s="1">
-        <v>1.9970000000000001E-3</v>
-      </c>
-      <c r="I35" s="1">
-        <v>1.9989999999999999E-3</v>
-      </c>
-      <c r="J35" s="1">
-        <v>3.9960000000000004E-3</v>
-      </c>
-      <c r="K35" s="1">
-        <v>1.9970000000000001E-3</v>
-      </c>
-      <c r="L35" s="1">
-        <v>6.9950000000000003E-3</v>
-      </c>
-      <c r="M35" s="1">
-        <v>1.5025999999999999E-2</v>
-      </c>
-      <c r="N35" s="1">
-        <v>4.0070000000000001E-3</v>
-      </c>
-      <c r="O35" s="1">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="P35" s="1">
-        <v>2.9949999999999998E-3</v>
-      </c>
-      <c r="Q35" s="1">
-        <v>1.9989999999999999E-3</v>
-      </c>
-      <c r="R35" s="1">
-        <v>6.0359999999999997E-3</v>
-      </c>
-      <c r="S35" s="1">
-        <v>8.9949999999999995E-3</v>
-      </c>
-      <c r="T35" s="1">
-        <v>2.5502E-2</v>
-      </c>
-      <c r="U35" s="1">
-        <v>5.9589999999999999E-3</v>
-      </c>
-      <c r="V35" s="6">
-        <v>1.3762E-2</v>
-      </c>
+      <c r="E41" s="2">
+        <v>0</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2">
+        <v>1.6333E-2</v>
+      </c>
+      <c r="H41" s="2">
+        <v>3.7810000000000001E-3</v>
+      </c>
+      <c r="I41" s="2">
+        <v>1.3389999999999999E-3</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0</v>
+      </c>
+      <c r="K41" s="2">
+        <v>8.8190000000000004E-3</v>
+      </c>
+      <c r="L41" s="2">
+        <v>6.391E-3</v>
+      </c>
+      <c r="M41" s="2">
+        <v>1.5242E-2</v>
+      </c>
+      <c r="N41" s="2">
+        <v>1.9090000000000001E-3</v>
+      </c>
+      <c r="O41" s="2">
+        <v>6.2570000000000004E-3</v>
+      </c>
+      <c r="P41" s="2">
+        <v>1.6429999999999999E-3</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>1.0169999999999999E-3</v>
+      </c>
+      <c r="R41" s="2">
+        <v>3.6949999999999999E-3</v>
+      </c>
+      <c r="S41" s="2">
+        <v>1.5363E-2</v>
+      </c>
+      <c r="T41" s="2">
+        <v>1.4251E-2</v>
+      </c>
+      <c r="U41" s="2">
+        <v>1.384E-2</v>
+      </c>
+      <c r="V41" s="8">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -27946,13 +28379,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C2644D-1F5F-4165-B7B9-8E10728AC7F6}">
   <dimension ref="C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q99" sqref="Q99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" s="10"/>
     </row>
   </sheetData>

</xml_diff>